<commit_message>
import tests + fixes in the parser
</commit_message>
<xml_diff>
--- a/curate/tests/data/parser/schema/namespace/tests.xlsx
+++ b/curate/tests/data/parser/schema/namespace/tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="25">
   <si>
     <t>qualified</t>
   </si>
@@ -85,16 +85,45 @@
   </si>
   <si>
     <t>mix qualified unqualified</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>Elements</t>
+  </si>
+  <si>
+    <t>Includes</t>
+  </si>
+  <si>
+    <t>Imports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,8 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +448,7 @@
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -445,27 +476,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -477,6 +513,9 @@
       </c>
       <c r="D9" t="s">
         <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G9">
         <v>1.1000000000000001</v>
@@ -490,8 +529,11 @@
       <c r="J9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9+1</f>
         <v>2</v>
@@ -505,6 +547,9 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G10">
         <f>G9+1</f>
         <v>2.1</v>
@@ -518,8 +563,11 @@
       <c r="J10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A50" si="0">A10+1</f>
         <v>3</v>
@@ -533,6 +581,9 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G11">
         <f t="shared" ref="G11:G16" si="1">G10+1</f>
         <v>3.1</v>
@@ -546,8 +597,11 @@
       <c r="J11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -560,6 +614,9 @@
       </c>
       <c r="D12" t="s">
         <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
@@ -574,8 +631,11 @@
       <c r="J12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -588,6 +648,9 @@
       </c>
       <c r="D13" t="s">
         <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
@@ -602,8 +665,11 @@
       <c r="J13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -616,6 +682,9 @@
       </c>
       <c r="D14" t="s">
         <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -630,8 +699,11 @@
       <c r="J14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -644,6 +716,9 @@
       </c>
       <c r="D15" t="s">
         <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
@@ -658,8 +733,11 @@
       <c r="J15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -672,6 +750,9 @@
       </c>
       <c r="D16" t="s">
         <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -686,8 +767,16 @@
       <c r="J16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -703,8 +792,12 @@
       <c r="E18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A18+1</f>
         <v>2</v>
@@ -721,8 +814,12 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -739,8 +836,12 @@
       <c r="E20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -757,8 +858,12 @@
       <c r="E21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -775,8 +880,11 @@
       <c r="E22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -793,8 +901,11 @@
       <c r="E23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -811,8 +922,11 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -829,8 +943,11 @@
       <c r="E25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -847,8 +964,11 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -865,8 +985,11 @@
       <c r="E27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -883,8 +1006,11 @@
       <c r="E28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -901,8 +1027,11 @@
       <c r="E29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -919,8 +1048,11 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -937,8 +1069,11 @@
       <c r="E31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -955,8 +1090,11 @@
       <c r="E32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -973,8 +1111,16 @@
       <c r="E33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -990,8 +1136,11 @@
       <c r="E35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A35+1</f>
         <v>2</v>
@@ -1008,8 +1157,11 @@
       <c r="E36" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1026,8 +1178,11 @@
       <c r="E37" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1044,8 +1199,11 @@
       <c r="E38" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1062,8 +1220,11 @@
       <c r="E39" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1080,8 +1241,11 @@
       <c r="E40" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1098,8 +1262,11 @@
       <c r="E41" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1116,8 +1283,11 @@
       <c r="E42" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1134,8 +1304,11 @@
       <c r="E43" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1152,8 +1325,11 @@
       <c r="E44" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1170,8 +1346,11 @@
       <c r="E45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1188,8 +1367,11 @@
       <c r="E46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1206,8 +1388,11 @@
       <c r="E47" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1224,8 +1409,11 @@
       <c r="E48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1242,8 +1430,11 @@
       <c r="E49" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1260,14 +1451,18 @@
       <c r="E50" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>